<commit_message>
Finishing the data mapper, @todo validate the entity record data by the entity constraint object
</commit_message>
<xml_diff>
--- a/resources/files/Master Data/hrd_bank.xlsx
+++ b/resources/files/Master Data/hrd_bank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsung\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\WebRoot\exporter\resources\files\Master Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>bank_code</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Bank Mandiri</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>Bank Central Asia</t>
   </si>
 </sst>
 </file>
@@ -354,9 +360,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -378,6 +386,14 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>